<commit_message>
Added Progress Report III (without hours)
</commit_message>
<xml_diff>
--- a/deliverables/Progress Reports/statistics.xlsx
+++ b/deliverables/Progress Reports/statistics.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9302"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="120" yWindow="120" windowWidth="24240" windowHeight="12075" activeTab="2"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="24">
   <si>
     <t>Sprint</t>
   </si>
@@ -294,10 +294,10 @@
                   <c:v>87</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>87</c:v>
+                  <c:v>6</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>87</c:v>
+                  <c:v>-2.5</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -314,11 +314,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="53515008"/>
-        <c:axId val="53516544"/>
+        <c:axId val="69828608"/>
+        <c:axId val="69830144"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="53515008"/>
+        <c:axId val="69828608"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -327,7 +327,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="53516544"/>
+        <c:crossAx val="69830144"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -335,7 +335,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="53516544"/>
+        <c:axId val="69830144"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -346,7 +346,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="53515008"/>
+        <c:crossAx val="69828608"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -356,6 +356,264 @@
       <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart10.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="en-CA"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:layout/>
+      <c:overlay val="0"/>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet3!$B$18</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Hours per Member</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>Sheet3!$A$19:$A$24</c:f>
+              <c:strCache>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>Cameron</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Glen</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Nick</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>Richard</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>James</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>Omar</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet3!$B$19:$B$24</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="1">
+                  <c:v>24.5</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>47.5</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>8</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="150"/>
+        <c:axId val="94870528"/>
+        <c:axId val="94968448"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="94870528"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="94968448"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="94968448"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="94870528"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart11.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="en-CA"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:layout/>
+      <c:overlay val="0"/>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:pieChart>
+        <c:varyColors val="1"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet3!$B$18</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Hours per Member</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:dLbls>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="0"/>
+            <c:showCatName val="1"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="1"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="1"/>
+          </c:dLbls>
+          <c:cat>
+            <c:strRef>
+              <c:f>Sheet3!$A$19:$A$24</c:f>
+              <c:strCache>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>Cameron</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Glen</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Nick</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>Richard</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>James</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>Omar</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet3!$B$19:$B$24</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="1">
+                  <c:v>24.5</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>47.5</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>8</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="1"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="1"/>
+          <c:showBubbleSize val="0"/>
+          <c:showLeaderLines val="1"/>
+        </c:dLbls>
+        <c:firstSliceAng val="0"/>
+      </c:pieChart>
+    </c:plotArea>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="gap"/>
     <c:showDLblsOverMax val="0"/>
@@ -447,22 +705,22 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
-                  <c:v>7.5</c:v>
+                  <c:v>8.3333333333333321</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>7</c:v>
+                  <c:v>17.5</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>6</c:v>
+                  <c:v>13</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>4</c:v>
+                  <c:v>10.833333333333332</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>4</c:v>
+                  <c:v>15.333333333333332</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>4.5</c:v>
+                  <c:v>10</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -507,7 +765,6 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:title>
     <c:autoTitleDeleted val="0"/>
@@ -571,22 +828,22 @@
                 <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
-                  <c:v>7.5</c:v>
+                  <c:v>10.5</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>4</c:v>
+                  <c:v>19</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>5</c:v>
+                  <c:v>19</c:v>
                 </c:pt>
                 <c:pt idx="3">
                   <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>4</c:v>
+                  <c:v>21.5</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>4.5</c:v>
+                  <c:v>5</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -644,11 +901,11 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet2!$B$12</c:f>
+              <c:f>Sheet2!$C$1</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>Expected Points</c:v>
+                  <c:v>Actual Points</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -664,7 +921,7 @@
           </c:dLbls>
           <c:cat>
             <c:strRef>
-              <c:f>Sheet2!$A$13:$A$18</c:f>
+              <c:f>Sheet2!$A$2:$A$7</c:f>
               <c:strCache>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
@@ -690,104 +947,27 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet2!$B$13:$B$18</c:f>
+              <c:f>Sheet2!$C$2:$C$7</c:f>
               <c:numCache>
-                <c:formatCode>General</c:formatCode>
+                <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
-                  <c:v>4</c:v>
+                  <c:v>10.5</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>9</c:v>
+                  <c:v>19</c:v>
                 </c:pt>
                 <c:pt idx="2">
+                  <c:v>19</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>21.5</c:v>
+                </c:pt>
+                <c:pt idx="5">
                   <c:v>5</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>4</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>4</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>4</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:val>
-        </c:ser>
-        <c:ser>
-          <c:idx val="1"/>
-          <c:order val="1"/>
-          <c:tx>
-            <c:strRef>
-              <c:f>Sheet2!$C$12</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>Actual Points</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:tx>
-          <c:dLbls>
-            <c:showLegendKey val="0"/>
-            <c:showVal val="0"/>
-            <c:showCatName val="1"/>
-            <c:showSerName val="0"/>
-            <c:showPercent val="1"/>
-            <c:showBubbleSize val="0"/>
-            <c:showLeaderLines val="1"/>
-          </c:dLbls>
-          <c:cat>
-            <c:strRef>
-              <c:f>Sheet2!$A$13:$A$18</c:f>
-              <c:strCache>
-                <c:ptCount val="6"/>
-                <c:pt idx="0">
-                  <c:v>Cameron</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>Glen</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>Nick</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>Richard</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>James</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>Omar</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:cat>
-          <c:val>
-            <c:numRef>
-              <c:f>Sheet2!$C$13:$C$18</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="6"/>
-                <c:pt idx="0">
-                  <c:v>0.5</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>8</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>4</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>1.5</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>0.5</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>13</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -832,7 +1012,6 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:title>
     <c:autoTitleDeleted val="0"/>
@@ -848,9 +1027,6 @@
               <c:f>Sheet2!$C$12</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>Actual Points</c:v>
-                </c:pt>
               </c:strCache>
             </c:strRef>
           </c:tx>
@@ -864,30 +1040,13 @@
             <c:showLeaderLines val="1"/>
           </c:dLbls>
           <c:cat>
-            <c:strRef>
+            <c:numRef>
               <c:f>Sheet2!$A$13:$A$18</c:f>
-              <c:strCache>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
                 <c:ptCount val="6"/>
-                <c:pt idx="0">
-                  <c:v>Cameron</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>Glen</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>Nick</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>Richard</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>James</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>Omar</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
+              </c:numCache>
+            </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
@@ -895,24 +1054,6 @@
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="6"/>
-                <c:pt idx="0">
-                  <c:v>0.5</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>8</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>4</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>1.5</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>0.5</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>13</c:v>
-                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
@@ -1044,11 +1185,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="107981824"/>
-        <c:axId val="96965376"/>
+        <c:axId val="82510976"/>
+        <c:axId val="82512512"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="107981824"/>
+        <c:axId val="82510976"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1057,14 +1198,15 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="96965376"/>
+        <c:crossAx val="82512512"/>
+        <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="96965376"/>
+        <c:axId val="82512512"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1075,7 +1217,8 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="107981824"/>
+        <c:crossAx val="82510976"/>
+        <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
     </c:plotArea>
@@ -1318,11 +1461,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="105625856"/>
-        <c:axId val="107134976"/>
+        <c:axId val="82554880"/>
+        <c:axId val="82556416"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="105625856"/>
+        <c:axId val="82554880"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1331,7 +1474,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="107134976"/>
+        <c:crossAx val="82556416"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1339,7 +1482,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="107134976"/>
+        <c:axId val="82556416"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1350,7 +1493,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="105625856"/>
+        <c:crossAx val="82554880"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1716,15 +1859,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>66675</xdr:colOff>
-      <xdr:row>18</xdr:row>
-      <xdr:rowOff>176212</xdr:rowOff>
+      <xdr:colOff>581025</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>52387</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>11</xdr:col>
-      <xdr:colOff>371475</xdr:colOff>
-      <xdr:row>33</xdr:row>
-      <xdr:rowOff>61912</xdr:rowOff>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>276225</xdr:colOff>
+      <xdr:row>30</xdr:row>
+      <xdr:rowOff>128587</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -1768,6 +1911,66 @@
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
           <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId4"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>547687</xdr:colOff>
+      <xdr:row>32</xdr:row>
+      <xdr:rowOff>57150</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>242887</xdr:colOff>
+      <xdr:row>46</xdr:row>
+      <xdr:rowOff>133350</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="6" name="Chart 5"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId5"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>538162</xdr:colOff>
+      <xdr:row>32</xdr:row>
+      <xdr:rowOff>133350</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>20</xdr:col>
+      <xdr:colOff>233362</xdr:colOff>
+      <xdr:row>47</xdr:row>
+      <xdr:rowOff>19050</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="7" name="Chart 6"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId6"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -2066,7 +2269,7 @@
   <dimension ref="A1:G9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+      <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2217,17 +2420,20 @@
         <f>56+29.5</f>
         <v>85.5</v>
       </c>
+      <c r="D6">
+        <v>81</v>
+      </c>
       <c r="E6">
         <f>B9-B2-B3-B4-B5-B6</f>
         <v>8.5</v>
       </c>
       <c r="F6">
         <f>B9-SUM(D2:D6)</f>
-        <v>87</v>
+        <v>6</v>
       </c>
       <c r="G6">
         <f t="shared" si="0"/>
-        <v>-78.5</v>
+        <v>2.5</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
@@ -2240,17 +2446,20 @@
       <c r="C7">
         <v>8.5</v>
       </c>
+      <c r="D7">
+        <v>8.5</v>
+      </c>
       <c r="E7">
         <f>B9-B2-B3-B4-B5-B6-B7</f>
         <v>0</v>
       </c>
       <c r="F7">
         <f>B9-SUM(D2:D7)</f>
-        <v>87</v>
+        <v>-2.5</v>
       </c>
       <c r="G7">
         <f t="shared" si="0"/>
-        <v>-87</v>
+        <v>2.5</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
@@ -2263,7 +2472,7 @@
       </c>
       <c r="D9">
         <f>SUM(D2:D7)</f>
-        <v>83.5</v>
+        <v>173</v>
       </c>
     </row>
   </sheetData>
@@ -2274,10 +2483,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C18"/>
+  <dimension ref="A1:C9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D22" sqref="D22"/>
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2302,11 +2511,12 @@
         <v>16</v>
       </c>
       <c r="B2">
-        <v>7.5</v>
+        <f>13/3+3/2+3/3+1+0.5</f>
+        <v>8.3333333333333321</v>
       </c>
       <c r="C2" s="1">
-        <f>3+3+0.5+5/6+1/6</f>
-        <v>7.5</v>
+        <f>13/2+3/2+3/2+3/3</f>
+        <v>10.5</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
@@ -2314,11 +2524,12 @@
         <v>17</v>
       </c>
       <c r="B3">
-        <v>7</v>
+        <f>8+1.5+1+3+3+1</f>
+        <v>17.5</v>
       </c>
       <c r="C3" s="1">
-        <f>1.5+1.5+5/6+1/6</f>
-        <v>4</v>
+        <f>8+3+1+3+3+1</f>
+        <v>19</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
@@ -2326,11 +2537,12 @@
         <v>18</v>
       </c>
       <c r="B4">
-        <v>6</v>
+        <f>4+2.5+1+3+1+0.5+1</f>
+        <v>13</v>
       </c>
       <c r="C4" s="1">
-        <f>3+1+5/6+1/6</f>
-        <v>5</v>
+        <f>8+5+1+3+1+0.25+0.25+0.25+0.25</f>
+        <v>19</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
@@ -2338,10 +2550,10 @@
         <v>19</v>
       </c>
       <c r="B5">
-        <v>4</v>
+        <f>4+13/3+1+1+0.5</f>
+        <v>10.833333333333332</v>
       </c>
       <c r="C5" s="1">
-        <f>5/6+1/6</f>
         <v>1</v>
       </c>
     </row>
@@ -2350,11 +2562,12 @@
         <v>20</v>
       </c>
       <c r="B6">
-        <v>4</v>
+        <f>3+4+13/3+3/2+3/3+0.5+0.5+0.5</f>
+        <v>15.333333333333332</v>
       </c>
       <c r="C6" s="1">
-        <f>3+5/6+1/6</f>
-        <v>4</v>
+        <f>3+8+13/2+3/2+3/2+1</f>
+        <v>21.5</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
@@ -2362,105 +2575,22 @@
         <v>21</v>
       </c>
       <c r="B7">
-        <v>4.5</v>
+        <f>4+2.5+1.5+1+0.5+0.5</f>
+        <v>10</v>
       </c>
       <c r="C7" s="1">
-        <f>0.5+1.5+1.5+1/6+5/6</f>
-        <v>4.5</v>
+        <f>5</f>
+        <v>5</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B9">
         <f>SUM(B2:B7)</f>
-        <v>33</v>
+        <v>74.999999999999986</v>
       </c>
       <c r="C9">
         <f>SUM(C2:C7)</f>
-        <v>26</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
-        <v>14</v>
-      </c>
-      <c r="B12" t="s">
-        <v>15</v>
-      </c>
-      <c r="C12" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
-        <v>16</v>
-      </c>
-      <c r="B13">
-        <f>4</f>
-        <v>4</v>
-      </c>
-      <c r="C13">
-        <f>0.5</f>
-        <v>0.5</v>
-      </c>
-    </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A14" t="s">
-        <v>17</v>
-      </c>
-      <c r="B14">
-        <v>9</v>
-      </c>
-      <c r="C14">
-        <f>3+5</f>
-        <v>8</v>
-      </c>
-    </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A15" t="s">
-        <v>18</v>
-      </c>
-      <c r="B15">
-        <v>5</v>
-      </c>
-      <c r="C15">
-        <f>1+1+1.5+0.5</f>
-        <v>4</v>
-      </c>
-    </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A16" t="s">
-        <v>19</v>
-      </c>
-      <c r="B16">
-        <v>4</v>
-      </c>
-      <c r="C16">
-        <f>1.5</f>
-        <v>1.5</v>
-      </c>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A17" t="s">
-        <v>20</v>
-      </c>
-      <c r="B17">
-        <v>4</v>
-      </c>
-      <c r="C17">
-        <f>0.5</f>
-        <v>0.5</v>
-      </c>
-    </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A18" t="s">
-        <v>21</v>
-      </c>
-      <c r="B18">
-        <v>4</v>
-      </c>
-      <c r="C18">
-        <f>5+8</f>
-        <v>13</v>
+        <v>76</v>
       </c>
     </row>
   </sheetData>
@@ -2471,10 +2601,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B16"/>
+  <dimension ref="A1:B24"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A10" sqref="A10:B16"/>
+    <sheetView tabSelected="1" topLeftCell="A5" workbookViewId="0">
+      <selection activeCell="A18" sqref="A18:B24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2594,6 +2724,53 @@
         <v>14</v>
       </c>
     </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>14</v>
+      </c>
+      <c r="B18" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>17</v>
+      </c>
+      <c r="B20">
+        <v>24.5</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>18</v>
+      </c>
+      <c r="B21">
+        <v>47.5</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>19</v>
+      </c>
+      <c r="B22">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>21</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>

</xml_diff>

<commit_message>
Added project final report.
</commit_message>
<xml_diff>
--- a/deliverables/Progress Reports/statistics.xlsx
+++ b/deliverables/Progress Reports/statistics.xlsx
@@ -1,22 +1,23 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9302"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="120" yWindow="120" windowWidth="24240" windowHeight="12075" activeTab="2"/>
+    <workbookView xWindow="120" yWindow="120" windowWidth="24240" windowHeight="12075" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
+    <sheet name="Sheet4" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="145621"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="25">
   <si>
     <t>Sprint</t>
   </si>
@@ -88,6 +89,9 @@
   </si>
   <si>
     <t>Hours per Member</t>
+  </si>
+  <si>
+    <t>Docs &amp; Demo</t>
   </si>
 </sst>
 </file>
@@ -314,11 +318,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="69828608"/>
-        <c:axId val="69830144"/>
+        <c:axId val="56440704"/>
+        <c:axId val="56442240"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="69828608"/>
+        <c:axId val="56440704"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -327,7 +331,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="69830144"/>
+        <c:crossAx val="56442240"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -335,7 +339,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="69830144"/>
+        <c:axId val="56442240"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -346,7 +350,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="69828608"/>
+        <c:crossAx val="56440704"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -440,6 +444,9 @@
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>30</c:v>
+                </c:pt>
                 <c:pt idx="1">
                   <c:v>24.5</c:v>
                 </c:pt>
@@ -448,6 +455,12 @@
                 </c:pt>
                 <c:pt idx="3">
                   <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>37</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>12</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -462,11 +475,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="94870528"/>
-        <c:axId val="94968448"/>
+        <c:axId val="82338176"/>
+        <c:axId val="82339712"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="94870528"/>
+        <c:axId val="82338176"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -475,7 +488,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="94968448"/>
+        <c:crossAx val="82339712"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -483,7 +496,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="94968448"/>
+        <c:axId val="82339712"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -494,7 +507,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="94870528"/>
+        <c:crossAx val="82338176"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -589,6 +602,9 @@
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>30</c:v>
+                </c:pt>
                 <c:pt idx="1">
                   <c:v>24.5</c:v>
                 </c:pt>
@@ -597,6 +613,12 @@
                 </c:pt>
                 <c:pt idx="3">
                   <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>37</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>12</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -614,6 +636,758 @@
         <c:firstSliceAng val="0"/>
       </c:pieChart>
     </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart12.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="en-CA"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet4!$B$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Nick</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:strRef>
+              <c:f>Sheet4!$A$2:$A$5</c:f>
+              <c:strCache>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>Webpage</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Batch</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Completion</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>Docs &amp; Demo</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet4!$B$2:$B$5</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>12</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>41.5</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>47.5</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet4!$C$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Cameron</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet4!$C$2:$C$5</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>15</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>30</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet4!$D$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Omar</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet4!$D$2:$D$5</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>14</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>14</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>12</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="3"/>
+          <c:order val="3"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet4!$E$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Glen</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet4!$E$2:$E$5</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>11</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>28.5</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>24.5</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="4"/>
+          <c:order val="4"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet4!$F$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>James</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet4!$F$2:$F$5</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>37</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="5"/>
+          <c:order val="5"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet4!$G$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Richard</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet4!$G$2:$G$5</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>8</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:marker val="1"/>
+        <c:smooth val="0"/>
+        <c:axId val="69221760"/>
+        <c:axId val="75821440"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="69221760"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="75821440"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="75821440"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="69221760"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:layout/>
+      <c:overlay val="0"/>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart13.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="en-CA"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet4!$B$8</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Nick</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:strRef>
+              <c:f>Sheet4!$A$9:$A$12</c:f>
+              <c:strCache>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>Webpage</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Batch</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Completion</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>Docs &amp; Demo</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet4!$B$9:$B$12</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>19</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet4!$C$8</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Cameron</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:strRef>
+              <c:f>Sheet4!$A$9:$A$12</c:f>
+              <c:strCache>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>Webpage</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Batch</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Completion</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>Docs &amp; Demo</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet4!$C$9:$C$12</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>7.5</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.5</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>10.5</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet4!$D$8</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Omar</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:strRef>
+              <c:f>Sheet4!$A$9:$A$12</c:f>
+              <c:strCache>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>Webpage</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Batch</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Completion</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>Docs &amp; Demo</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet4!$D$9:$D$12</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>4.5</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>13</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>5</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="3"/>
+          <c:order val="3"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet4!$E$8</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Glen</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:strRef>
+              <c:f>Sheet4!$A$9:$A$12</c:f>
+              <c:strCache>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>Webpage</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Batch</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Completion</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>Docs &amp; Demo</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet4!$E$9:$E$12</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>19</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="4"/>
+          <c:order val="4"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet4!$F$8</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>James</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:strRef>
+              <c:f>Sheet4!$A$9:$A$12</c:f>
+              <c:strCache>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>Webpage</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Batch</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Completion</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>Docs &amp; Demo</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet4!$F$9:$F$12</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.5</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>21.5</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="5"/>
+          <c:order val="5"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet4!$G$8</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Richard</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:strRef>
+              <c:f>Sheet4!$A$9:$A$12</c:f>
+              <c:strCache>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>Webpage</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Batch</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Completion</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>Docs &amp; Demo</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet4!$G$9:$G$12</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1.5</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:marker val="1"/>
+        <c:smooth val="0"/>
+        <c:axId val="110202880"/>
+        <c:axId val="110204416"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="110202880"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="110204416"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="110204416"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="110202880"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:layout/>
+      <c:overlay val="0"/>
+    </c:legend>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="gap"/>
     <c:showDLblsOverMax val="0"/>
@@ -765,6 +1539,7 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
+      <c:layout/>
       <c:overlay val="0"/>
     </c:title>
     <c:autoTitleDeleted val="0"/>
@@ -1012,6 +1787,7 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
+      <c:layout/>
       <c:overlay val="0"/>
     </c:title>
     <c:autoTitleDeleted val="0"/>
@@ -1185,11 +1961,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="82510976"/>
-        <c:axId val="82512512"/>
+        <c:axId val="81262080"/>
+        <c:axId val="81263616"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="82510976"/>
+        <c:axId val="81262080"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1198,7 +1974,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="82512512"/>
+        <c:crossAx val="81263616"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1206,7 +1982,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="82512512"/>
+        <c:axId val="81263616"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1217,7 +1993,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="82510976"/>
+        <c:crossAx val="81262080"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1461,11 +2237,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="82554880"/>
-        <c:axId val="82556416"/>
+        <c:axId val="81953536"/>
+        <c:axId val="81955072"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="82554880"/>
+        <c:axId val="81953536"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1474,7 +2250,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="82556416"/>
+        <c:crossAx val="81955072"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1482,7 +2258,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="82556416"/>
+        <c:axId val="81955072"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1493,7 +2269,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="82554880"/>
+        <c:crossAx val="81953536"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1979,6 +2755,73 @@
 </xdr:wsDr>
 </file>
 
+<file path=xl/drawings/drawing4.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>123825</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>428625</xdr:colOff>
+      <xdr:row>12</xdr:row>
+      <xdr:rowOff>76200</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="4" name="Chart 3"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>133350</xdr:colOff>
+      <xdr:row>13</xdr:row>
+      <xdr:rowOff>9525</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>438150</xdr:colOff>
+      <xdr:row>27</xdr:row>
+      <xdr:rowOff>85725</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="6" name="Chart 5"/>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
 <a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
@@ -2269,7 +3112,7 @@
   <dimension ref="A1:G9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D8" sqref="D8"/>
+      <selection activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2486,7 +3329,7 @@
   <dimension ref="A1:C9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+      <selection activeCell="B24" sqref="B24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2603,8 +3446,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B24"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A5" workbookViewId="0">
-      <selection activeCell="A18" sqref="A18:B24"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C51" sqref="C51"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2736,6 +3579,9 @@
       <c r="A19" t="s">
         <v>16</v>
       </c>
+      <c r="B19">
+        <v>30</v>
+      </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
@@ -2765,10 +3611,229 @@
       <c r="A23" t="s">
         <v>20</v>
       </c>
+      <c r="B23">
+        <v>37</v>
+      </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>21</v>
+      </c>
+      <c r="B24">
+        <v>12</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:G12"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F18" sqref="F18"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="12.7109375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>18</v>
+      </c>
+      <c r="C1" t="s">
+        <v>16</v>
+      </c>
+      <c r="D1" t="s">
+        <v>21</v>
+      </c>
+      <c r="E1" t="s">
+        <v>17</v>
+      </c>
+      <c r="F1" t="s">
+        <v>20</v>
+      </c>
+      <c r="G1" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2">
+        <v>12</v>
+      </c>
+      <c r="C2">
+        <v>6</v>
+      </c>
+      <c r="D2">
+        <v>14</v>
+      </c>
+      <c r="E2">
+        <v>11</v>
+      </c>
+      <c r="F2">
+        <v>8</v>
+      </c>
+      <c r="G2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>2</v>
+      </c>
+      <c r="B3">
+        <v>41.5</v>
+      </c>
+      <c r="C3">
+        <v>15</v>
+      </c>
+      <c r="D3">
+        <v>14</v>
+      </c>
+      <c r="E3">
+        <v>28.5</v>
+      </c>
+      <c r="F3">
+        <v>16</v>
+      </c>
+      <c r="G3">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>5</v>
+      </c>
+      <c r="B4">
+        <v>47.5</v>
+      </c>
+      <c r="C4">
+        <v>30</v>
+      </c>
+      <c r="D4">
+        <v>12</v>
+      </c>
+      <c r="E4">
+        <v>24.5</v>
+      </c>
+      <c r="F4">
+        <v>37</v>
+      </c>
+      <c r="G4">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>0</v>
+      </c>
+      <c r="B8" t="s">
+        <v>18</v>
+      </c>
+      <c r="C8" t="s">
+        <v>16</v>
+      </c>
+      <c r="D8" t="s">
+        <v>21</v>
+      </c>
+      <c r="E8" t="s">
+        <v>17</v>
+      </c>
+      <c r="F8" t="s">
+        <v>20</v>
+      </c>
+      <c r="G8" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>1</v>
+      </c>
+      <c r="B9">
+        <v>5</v>
+      </c>
+      <c r="C9">
+        <v>7.5</v>
+      </c>
+      <c r="D9">
+        <v>4.5</v>
+      </c>
+      <c r="E9">
+        <v>4</v>
+      </c>
+      <c r="F9">
+        <v>4</v>
+      </c>
+      <c r="G9">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>2</v>
+      </c>
+      <c r="B10">
+        <v>4</v>
+      </c>
+      <c r="C10">
+        <v>0.5</v>
+      </c>
+      <c r="D10">
+        <v>13</v>
+      </c>
+      <c r="E10">
+        <v>8</v>
+      </c>
+      <c r="F10">
+        <v>0.5</v>
+      </c>
+      <c r="G10">
+        <v>1.5</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>5</v>
+      </c>
+      <c r="B11">
+        <v>19</v>
+      </c>
+      <c r="C11">
+        <v>10.5</v>
+      </c>
+      <c r="D11">
+        <v>5</v>
+      </c>
+      <c r="E11">
+        <v>19</v>
+      </c>
+      <c r="F11">
+        <v>21.5</v>
+      </c>
+      <c r="G11">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>24</v>
       </c>
     </row>
   </sheetData>

</xml_diff>